<commit_message>
Moved achievements to a different thread -> using asynchronous functions to process the data!
</commit_message>
<xml_diff>
--- a/static.xlsx
+++ b/static.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual Java\Gw2 Discord Bot\gw2discordbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3CB926-266D-437E-8A2A-5C090A9772EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6855D16E-4AF9-432E-A65F-138FAF48EBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4710" yWindow="2625" windowWidth="23490" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Signups" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="66">
   <si>
     <t>EMPTY</t>
   </si>
@@ -176,6 +176,51 @@
   </si>
   <si>
     <t>FILL</t>
+  </si>
+  <si>
+    <t>448782054893813780</t>
+  </si>
+  <si>
+    <t>345926812976545792</t>
+  </si>
+  <si>
+    <t>345325716599996416</t>
+  </si>
+  <si>
+    <t>185066811732000768</t>
+  </si>
+  <si>
+    <t>163239274127425536</t>
+  </si>
+  <si>
+    <t>471044613596250121</t>
+  </si>
+  <si>
+    <t>209629323366367232</t>
+  </si>
+  <si>
+    <t>HAM (TANK)</t>
+  </si>
+  <si>
+    <t>HAM / AlacMech / Heal Alac Druid</t>
+  </si>
+  <si>
+    <t>QFB [MAIN] (SH TANK) / Qscrapper</t>
+  </si>
+  <si>
+    <t>Qscrapper [MAIN] / QFB</t>
+  </si>
+  <si>
+    <t>Mesmer / Q6 Kite</t>
+  </si>
+  <si>
+    <t>DPS [MAIN] / HK / Lamp / Pylon</t>
+  </si>
+  <si>
+    <t>DPS [MAIN] / EPI / Q6 Mesmer / Pylon</t>
+  </si>
+  <si>
+    <t>DPS [MAIN] / Lamp / Pylon</t>
   </si>
 </sst>
 </file>
@@ -614,7 +659,9 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -626,34 +673,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -661,28 +708,28 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>12</v>
@@ -1758,9 +1805,7 @@
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>